<commit_message>
Banco Central - RESOLUÇÃO Nº 4.658, DE 26 DE ABRIL DE 2018
RESOLUÇÃO Nº 4.658, DE 26 DE ABRIL DE 2018

Dispõe sobre a política de segurança cibernética e sobre os requisitos para a contratação de serviços de processamento e armazenamento de dados e de computação em nuvem a serem observados pelas instituições financeiras e demais instituições autorizadas a funcionar pelo Banco Central do Brasil.
O Banco Central do Brasil, na forma do art. 9º da Lei nº 4.595, de 31 de dezembro de 1964, torna público que o Conselho Monetário Nacional, em sessão realizada em 26 de abril de 2018, com base nos arts. 4º, inciso VIII, da referida Lei, 9º da Lei nº 4.728, de 14 de julho de 1965, 7º e 23, alínea "a", da Lei nº 6.099, de 12 de setembro de 1974, 1º, inciso II, da Lei nº 10.194, de 14 de fevereiro de 2001, e 1º, § 1º, da Lei Complementar nº 130, de 17 de abril de 2009,
</commit_message>
<xml_diff>
--- a/LGPD.xlsx
+++ b/LGPD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hackti-my.sharepoint.com/personal/pedro_bezerra_hackti_org/Documents/DEV/Dev_Watson/Bases_para_Github/Bases-de-Dados-de-GRC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive_HackTi.org\OneDrive - Hackti.org\DEV\Dev_Watson\Bases_para_Github\Bases-de-Dados-de-GRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{CCF31137-B40F-40A9-974F-918B553C718A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{63A1961E-ADC7-4724-88CD-6BD6F549B852}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{CCF31137-B40F-40A9-974F-918B553C718A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CF33EE0D-5D29-45F3-A508-35BC4A9F5C13}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="8820" activeTab="1" xr2:uid="{146E37C3-4AEE-4B0F-9DAE-2D73837273AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="8820" xr2:uid="{146E37C3-4AEE-4B0F-9DAE-2D73837273AB}"/>
   </bookViews>
   <sheets>
     <sheet name="LGPD_Integra" sheetId="2" r:id="rId1"/>
@@ -10476,8 +10476,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1269</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1020444</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>874394</xdr:rowOff>
     </xdr:to>
@@ -10820,11 +10820,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E13DC0-796A-4D80-B2CA-08AE85BB4F8F}">
   <dimension ref="A1:A471"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="56.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="1.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="3.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
@@ -13205,7 +13207,7 @@
   </sheetPr>
   <dimension ref="A1:D385"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>